<commit_message>
Re-run analyses due to tiny mistake and inclusion of even more data
</commit_message>
<xml_diff>
--- a/Names.xlsx
+++ b/Names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\GitHub\Ischnura_Reinforcement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C28EBB-D7AC-4E62-8A30-6C831EE9717B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2153AAD4-7BA1-4132-AA48-BD8D56769A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A9BA1AB8-E61D-4C57-8F87-AFE6D9DBAD1E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Population</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>AGra</t>
+  </si>
+  <si>
+    <t>Riomaior</t>
+  </si>
+  <si>
+    <t>Rio</t>
   </si>
 </sst>
 </file>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43394BDD-7C40-49A1-B13E-355682881545}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,25 +643,33 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>